<commit_message>
Worked on prac write tut
</commit_message>
<xml_diff>
--- a/prac/pracdatasheet.xlsx
+++ b/prac/pracdatasheet.xlsx
@@ -10029,7 +10029,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -10043,6 +10043,11 @@
       <sz val="8.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="8.0"/>
@@ -10070,7 +10075,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -10084,26 +10089,29 @@
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -10378,7 +10386,9 @@
       <c r="C2" s="3">
         <v>0.0</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4">
+        <v>4.6</v>
+      </c>
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
@@ -10399,7 +10409,9 @@
       <c r="C3" s="3">
         <v>5.0</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4">
+        <v>5.4</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
@@ -10420,7 +10432,9 @@
       <c r="C4" s="3">
         <v>0.0</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4">
+        <v>3.79</v>
+      </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
@@ -10441,7 +10455,9 @@
       <c r="C5" s="3">
         <v>10.0</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4">
+        <v>4.82</v>
+      </c>
       <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
@@ -10462,7 +10478,9 @@
       <c r="C6" s="3">
         <v>5.0</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4">
+        <v>4.91</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
@@ -10483,7 +10501,9 @@
       <c r="C7" s="3">
         <v>0.0</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4">
+        <v>6.48</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
@@ -10504,7 +10524,9 @@
       <c r="C8" s="3">
         <v>0.0</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4">
+        <v>5.13</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>19</v>
       </c>
@@ -10525,7 +10547,9 @@
       <c r="C9" s="3">
         <v>30.0</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4">
+        <v>5.7</v>
+      </c>
       <c r="E9" s="2" t="s">
         <v>20</v>
       </c>
@@ -10544,9 +10568,11 @@
         <v>18</v>
       </c>
       <c r="C10" s="3">
-        <v>25.0</v>
-      </c>
-      <c r="D10" s="4"/>
+        <v>5.0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>3.7</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>21</v>
       </c>
@@ -10567,7 +10593,9 @@
       <c r="C11" s="3">
         <v>8.0</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="4">
+        <v>4.54</v>
+      </c>
       <c r="E11" s="2" t="s">
         <v>22</v>
       </c>
@@ -10588,7 +10616,9 @@
       <c r="C12" s="3">
         <v>45.0</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="4">
+        <v>4.72</v>
+      </c>
       <c r="E12" s="2" t="s">
         <v>19</v>
       </c>
@@ -10609,7 +10639,9 @@
       <c r="C13" s="3">
         <v>40.0</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="4">
+        <v>6.08</v>
+      </c>
       <c r="E13" s="2" t="s">
         <v>23</v>
       </c>
@@ -10630,7 +10662,9 @@
       <c r="C14" s="5">
         <v>0.0</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="4">
+        <v>5.11</v>
+      </c>
       <c r="E14" s="2" t="s">
         <v>25</v>
       </c>
@@ -10651,7 +10685,9 @@
       <c r="C15" s="5">
         <v>20.0</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="4">
+        <v>5.43</v>
+      </c>
       <c r="E15" s="2" t="s">
         <v>26</v>
       </c>
@@ -10670,9 +10706,11 @@
         <v>24</v>
       </c>
       <c r="C16" s="3">
-        <v>90.0</v>
-      </c>
-      <c r="D16" s="4"/>
+        <v>10.0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3.93</v>
+      </c>
       <c r="E16" s="2" t="s">
         <v>27</v>
       </c>
@@ -10693,7 +10731,9 @@
       <c r="C17" s="3">
         <v>20.0</v>
       </c>
-      <c r="D17" s="4"/>
+      <c r="D17" s="4">
+        <v>4.94</v>
+      </c>
       <c r="E17" s="2" t="s">
         <v>15</v>
       </c>
@@ -10714,7 +10754,9 @@
       <c r="C18" s="3">
         <v>30.0</v>
       </c>
-      <c r="D18" s="4"/>
+      <c r="D18" s="4">
+        <v>4.7</v>
+      </c>
       <c r="E18" s="2" t="s">
         <v>11</v>
       </c>
@@ -10735,7 +10777,9 @@
       <c r="C19" s="3">
         <v>40.0</v>
       </c>
-      <c r="D19" s="4"/>
+      <c r="D19" s="4">
+        <v>6.3</v>
+      </c>
       <c r="E19" s="2" t="s">
         <v>11</v>
       </c>
@@ -10756,7 +10800,9 @@
       <c r="C20" s="3">
         <v>10.0</v>
       </c>
-      <c r="D20" s="4"/>
+      <c r="D20" s="4">
+        <v>4.57</v>
+      </c>
       <c r="E20" s="2" t="s">
         <v>29</v>
       </c>
@@ -10777,7 +10823,9 @@
       <c r="C21" s="3">
         <v>30.0</v>
       </c>
-      <c r="D21" s="4"/>
+      <c r="D21" s="4">
+        <v>5.35</v>
+      </c>
       <c r="E21" s="2" t="s">
         <v>30</v>
       </c>
@@ -10796,9 +10844,11 @@
         <v>28</v>
       </c>
       <c r="C22" s="3">
-        <v>90.0</v>
-      </c>
-      <c r="D22" s="4"/>
+        <v>5.0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>4.1</v>
+      </c>
       <c r="E22" s="2" t="s">
         <v>31</v>
       </c>
@@ -10819,7 +10869,9 @@
       <c r="C23" s="3">
         <v>10.0</v>
       </c>
-      <c r="D23" s="4"/>
+      <c r="D23" s="4">
+        <v>4.95</v>
+      </c>
       <c r="E23" s="2" t="s">
         <v>32</v>
       </c>
@@ -10840,7 +10892,9 @@
       <c r="C24" s="3">
         <v>45.0</v>
       </c>
-      <c r="D24" s="4"/>
+      <c r="D24" s="4">
+        <v>4.7</v>
+      </c>
       <c r="E24" s="2" t="s">
         <v>33</v>
       </c>
@@ -10861,7 +10915,9 @@
       <c r="C25" s="3">
         <v>40.0</v>
       </c>
-      <c r="D25" s="4"/>
+      <c r="D25" s="4">
+        <v>6.45</v>
+      </c>
       <c r="E25" s="2" t="s">
         <v>34</v>
       </c>
@@ -18692,7 +18748,7 @@
     <dataValidation type="list" allowBlank="1" sqref="B1:B1000">
       <formula1>RangeLimits!$B$1:$B$4</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showDropDown="1" sqref="D1:D1000">
+    <dataValidation type="decimal" allowBlank="1" showDropDown="1" sqref="D1 D26:D1000">
       <formula1>0.0</formula1>
       <formula2>14.0</formula2>
     </dataValidation>
@@ -19421,7 +19477,7 @@
       <c r="F20" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="4"/>
+      <c r="G20" s="7"/>
       <c r="H20" s="3">
         <v>50.0</v>
       </c>
@@ -19455,7 +19511,7 @@
       <c r="F21" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G21" s="4"/>
+      <c r="G21" s="7"/>
       <c r="H21" s="3">
         <v>40.0</v>
       </c>
@@ -19489,7 +19545,7 @@
       <c r="F22" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="4"/>
+      <c r="G22" s="7"/>
       <c r="H22" s="3">
         <v>58.0</v>
       </c>
@@ -19847,7 +19903,7 @@
       <c r="F32" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G32" s="4"/>
+      <c r="G32" s="7"/>
       <c r="H32" s="3">
         <v>300.0</v>
       </c>
@@ -19881,7 +19937,7 @@
       <c r="F33" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G33" s="4"/>
+      <c r="G33" s="7"/>
       <c r="H33" s="3">
         <v>280.0</v>
       </c>
@@ -19915,7 +19971,7 @@
       <c r="F34" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G34" s="4"/>
+      <c r="G34" s="7"/>
       <c r="H34" s="3">
         <v>140.0</v>
       </c>
@@ -20255,154 +20311,154 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="8">
+      <c r="C44" s="9">
         <v>4.0</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D44" s="9">
         <v>1.0</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E44" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="F44" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G44" s="9"/>
-      <c r="H44" s="8">
+      <c r="G44" s="10"/>
+      <c r="H44" s="9">
         <v>92.0</v>
       </c>
-      <c r="I44" s="8">
+      <c r="I44" s="9">
         <v>4.31</v>
       </c>
-      <c r="J44" s="8">
+      <c r="J44" s="9">
         <v>2.2</v>
       </c>
       <c r="K44" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Bruniaceae </v>
       </c>
-      <c r="L44" s="10"/>
-      <c r="M44" s="10"/>
-      <c r="N44" s="10"/>
-      <c r="O44" s="10"/>
-      <c r="P44" s="10"/>
-      <c r="Q44" s="10"/>
-      <c r="R44" s="10"/>
-      <c r="S44" s="10"/>
-      <c r="T44" s="10"/>
-      <c r="U44" s="10"/>
-      <c r="V44" s="10"/>
-      <c r="W44" s="10"/>
-      <c r="X44" s="10"/>
-      <c r="Y44" s="10"/>
-      <c r="Z44" s="10"/>
-      <c r="AA44" s="10"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11"/>
+      <c r="T44" s="11"/>
+      <c r="U44" s="11"/>
+      <c r="V44" s="11"/>
+      <c r="W44" s="11"/>
+      <c r="X44" s="11"/>
+      <c r="Y44" s="11"/>
+      <c r="Z44" s="11"/>
+      <c r="AA44" s="11"/>
     </row>
     <row r="45">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C45" s="8">
+      <c r="C45" s="9">
         <v>4.0</v>
       </c>
-      <c r="D45" s="8">
+      <c r="D45" s="9">
         <v>2.0</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="E45" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="F45" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G45" s="9"/>
-      <c r="H45" s="8">
+      <c r="G45" s="10"/>
+      <c r="H45" s="9">
         <v>113.0</v>
       </c>
-      <c r="I45" s="8">
+      <c r="I45" s="9">
         <v>4.42</v>
       </c>
-      <c r="J45" s="8">
+      <c r="J45" s="9">
         <v>2.46</v>
       </c>
       <c r="K45" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Bruniaceae </v>
       </c>
-      <c r="L45" s="10"/>
-      <c r="M45" s="10"/>
-      <c r="N45" s="10"/>
-      <c r="O45" s="10"/>
-      <c r="P45" s="10"/>
-      <c r="Q45" s="10"/>
-      <c r="R45" s="10"/>
-      <c r="S45" s="10"/>
-      <c r="T45" s="10"/>
-      <c r="U45" s="10"/>
-      <c r="V45" s="10"/>
-      <c r="W45" s="10"/>
-      <c r="X45" s="10"/>
-      <c r="Y45" s="10"/>
-      <c r="Z45" s="10"/>
-      <c r="AA45" s="10"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+      <c r="T45" s="11"/>
+      <c r="U45" s="11"/>
+      <c r="V45" s="11"/>
+      <c r="W45" s="11"/>
+      <c r="X45" s="11"/>
+      <c r="Y45" s="11"/>
+      <c r="Z45" s="11"/>
+      <c r="AA45" s="11"/>
     </row>
     <row r="46">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C46" s="8">
+      <c r="C46" s="9">
         <v>4.0</v>
       </c>
-      <c r="D46" s="8">
+      <c r="D46" s="9">
         <v>3.0</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E46" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F46" s="7" t="s">
+      <c r="F46" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G46" s="9"/>
-      <c r="H46" s="8">
+      <c r="G46" s="10"/>
+      <c r="H46" s="9">
         <v>164.0</v>
       </c>
-      <c r="I46" s="8">
+      <c r="I46" s="9">
         <v>5.04</v>
       </c>
-      <c r="J46" s="8">
+      <c r="J46" s="9">
         <v>1.86</v>
       </c>
       <c r="K46" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Bruniaceae </v>
       </c>
-      <c r="L46" s="10"/>
-      <c r="M46" s="10"/>
-      <c r="N46" s="10"/>
-      <c r="O46" s="10"/>
-      <c r="P46" s="10"/>
-      <c r="Q46" s="10"/>
-      <c r="R46" s="10"/>
-      <c r="S46" s="10"/>
-      <c r="T46" s="10"/>
-      <c r="U46" s="10"/>
-      <c r="V46" s="10"/>
-      <c r="W46" s="10"/>
-      <c r="X46" s="10"/>
-      <c r="Y46" s="10"/>
-      <c r="Z46" s="10"/>
-      <c r="AA46" s="10"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="11"/>
+      <c r="R46" s="11"/>
+      <c r="S46" s="11"/>
+      <c r="T46" s="11"/>
+      <c r="U46" s="11"/>
+      <c r="V46" s="11"/>
+      <c r="W46" s="11"/>
+      <c r="X46" s="11"/>
+      <c r="Y46" s="11"/>
+      <c r="Z46" s="11"/>
+      <c r="AA46" s="11"/>
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
@@ -20531,7 +20587,7 @@
       <c r="F50" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G50" s="4"/>
+      <c r="G50" s="7"/>
       <c r="H50" s="3">
         <v>140.0</v>
       </c>
@@ -20565,7 +20621,7 @@
       <c r="F51" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G51" s="4"/>
+      <c r="G51" s="7"/>
       <c r="H51" s="3">
         <v>110.0</v>
       </c>
@@ -20599,7 +20655,7 @@
       <c r="F52" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G52" s="4"/>
+      <c r="G52" s="7"/>
       <c r="H52" s="3">
         <v>130.0</v>
       </c>
@@ -20849,7 +20905,7 @@
       <c r="F59" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G59" s="4"/>
+      <c r="G59" s="7"/>
       <c r="H59" s="3">
         <v>120.0</v>
       </c>
@@ -20883,7 +20939,7 @@
       <c r="F60" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G60" s="4"/>
+      <c r="G60" s="7"/>
       <c r="H60" s="3">
         <v>100.0</v>
       </c>
@@ -20917,7 +20973,7 @@
       <c r="F61" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G61" s="4"/>
+      <c r="G61" s="7"/>
       <c r="H61" s="3">
         <v>100.0</v>
       </c>
@@ -21167,7 +21223,7 @@
       <c r="F68" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G68" s="4"/>
+      <c r="G68" s="7"/>
       <c r="H68" s="3">
         <v>90.0</v>
       </c>
@@ -21201,7 +21257,7 @@
       <c r="F69" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G69" s="4"/>
+      <c r="G69" s="7"/>
       <c r="H69" s="3">
         <v>70.0</v>
       </c>
@@ -21235,7 +21291,7 @@
       <c r="F70" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G70" s="4"/>
+      <c r="G70" s="7"/>
       <c r="H70" s="3">
         <v>80.0</v>
       </c>
@@ -21269,7 +21325,7 @@
       <c r="F71" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G71" s="4"/>
+      <c r="G71" s="7"/>
       <c r="H71" s="3">
         <v>200.0</v>
       </c>
@@ -21303,7 +21359,7 @@
       <c r="F72" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G72" s="4"/>
+      <c r="G72" s="7"/>
       <c r="H72" s="3">
         <v>130.0</v>
       </c>
@@ -21337,7 +21393,7 @@
       <c r="F73" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G73" s="4"/>
+      <c r="G73" s="7"/>
       <c r="H73" s="3">
         <v>90.0</v>
       </c>
@@ -21371,7 +21427,7 @@
       <c r="F74" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G74" s="4"/>
+      <c r="G74" s="7"/>
       <c r="H74" s="3">
         <v>70.0</v>
       </c>
@@ -21405,7 +21461,7 @@
       <c r="F75" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G75" s="4"/>
+      <c r="G75" s="7"/>
       <c r="H75" s="3">
         <v>100.0</v>
       </c>
@@ -21439,7 +21495,7 @@
       <c r="F76" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G76" s="4"/>
+      <c r="G76" s="7"/>
       <c r="H76" s="3">
         <v>85.0</v>
       </c>
@@ -21473,7 +21529,7 @@
       <c r="F77" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G77" s="4"/>
+      <c r="G77" s="7"/>
       <c r="H77" s="3">
         <v>45.0</v>
       </c>
@@ -21507,7 +21563,7 @@
       <c r="F78" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G78" s="4"/>
+      <c r="G78" s="7"/>
       <c r="H78" s="3">
         <v>60.0</v>
       </c>
@@ -21541,7 +21597,7 @@
       <c r="F79" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G79" s="4"/>
+      <c r="G79" s="7"/>
       <c r="H79" s="3">
         <v>30.0</v>
       </c>
@@ -21791,7 +21847,7 @@
       <c r="F86" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G86" s="4"/>
+      <c r="G86" s="7"/>
       <c r="H86" s="3">
         <v>355.0</v>
       </c>
@@ -21825,7 +21881,7 @@
       <c r="F87" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G87" s="4"/>
+      <c r="G87" s="7"/>
       <c r="H87" s="3">
         <v>515.0</v>
       </c>
@@ -21859,7 +21915,7 @@
       <c r="F88" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G88" s="4"/>
+      <c r="G88" s="7"/>
       <c r="H88" s="3">
         <v>413.0</v>
       </c>
@@ -21893,7 +21949,7 @@
       <c r="F89" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G89" s="4"/>
+      <c r="G89" s="7"/>
       <c r="H89" s="3">
         <v>550.0</v>
       </c>
@@ -21927,7 +21983,7 @@
       <c r="F90" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G90" s="4"/>
+      <c r="G90" s="7"/>
       <c r="H90" s="3">
         <v>480.0</v>
       </c>
@@ -21961,7 +22017,7 @@
       <c r="F91" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G91" s="4"/>
+      <c r="G91" s="7"/>
       <c r="H91" s="3">
         <v>500.0</v>
       </c>
@@ -22211,7 +22267,7 @@
       <c r="F98" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G98" s="4"/>
+      <c r="G98" s="7"/>
       <c r="H98" s="3">
         <v>510.0</v>
       </c>
@@ -22245,7 +22301,7 @@
       <c r="F99" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G99" s="4"/>
+      <c r="G99" s="7"/>
       <c r="H99" s="3">
         <v>580.0</v>
       </c>
@@ -22279,7 +22335,7 @@
       <c r="F100" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G100" s="4"/>
+      <c r="G100" s="7"/>
       <c r="H100" s="3">
         <v>350.0</v>
       </c>
@@ -22295,154 +22351,154 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="7" t="s">
+      <c r="A101" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B101" s="7" t="s">
+      <c r="B101" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C101" s="8">
+      <c r="C101" s="9">
         <v>1.0</v>
       </c>
-      <c r="D101" s="8">
+      <c r="D101" s="9">
         <v>1.0</v>
       </c>
-      <c r="E101" s="7" t="s">
+      <c r="E101" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="F101" s="7" t="s">
+      <c r="F101" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="G101" s="9"/>
-      <c r="H101" s="8">
+      <c r="G101" s="10"/>
+      <c r="H101" s="9">
         <v>144.0</v>
       </c>
-      <c r="I101" s="8">
+      <c r="I101" s="9">
         <v>66.99</v>
       </c>
-      <c r="J101" s="8">
+      <c r="J101" s="9">
         <v>2.38</v>
       </c>
       <c r="K101" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Restio </v>
       </c>
-      <c r="L101" s="10"/>
-      <c r="M101" s="10"/>
-      <c r="N101" s="10"/>
-      <c r="O101" s="10"/>
-      <c r="P101" s="10"/>
-      <c r="Q101" s="10"/>
-      <c r="R101" s="10"/>
-      <c r="S101" s="10"/>
-      <c r="T101" s="10"/>
-      <c r="U101" s="10"/>
-      <c r="V101" s="10"/>
-      <c r="W101" s="10"/>
-      <c r="X101" s="10"/>
-      <c r="Y101" s="10"/>
-      <c r="Z101" s="10"/>
-      <c r="AA101" s="10"/>
+      <c r="L101" s="11"/>
+      <c r="M101" s="11"/>
+      <c r="N101" s="11"/>
+      <c r="O101" s="11"/>
+      <c r="P101" s="11"/>
+      <c r="Q101" s="11"/>
+      <c r="R101" s="11"/>
+      <c r="S101" s="11"/>
+      <c r="T101" s="11"/>
+      <c r="U101" s="11"/>
+      <c r="V101" s="11"/>
+      <c r="W101" s="11"/>
+      <c r="X101" s="11"/>
+      <c r="Y101" s="11"/>
+      <c r="Z101" s="11"/>
+      <c r="AA101" s="11"/>
     </row>
     <row r="102">
-      <c r="A102" s="7" t="s">
+      <c r="A102" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B102" s="7" t="s">
+      <c r="B102" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C102" s="8">
+      <c r="C102" s="9">
         <v>1.0</v>
       </c>
-      <c r="D102" s="8">
+      <c r="D102" s="9">
         <v>2.0</v>
       </c>
-      <c r="E102" s="7" t="s">
+      <c r="E102" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="F102" s="7" t="s">
+      <c r="F102" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="G102" s="9"/>
-      <c r="H102" s="8">
+      <c r="G102" s="10"/>
+      <c r="H102" s="9">
         <v>180.0</v>
       </c>
-      <c r="I102" s="8">
+      <c r="I102" s="9">
         <v>37.33</v>
       </c>
-      <c r="J102" s="8">
+      <c r="J102" s="9">
         <v>1.13</v>
       </c>
       <c r="K102" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Restio </v>
       </c>
-      <c r="L102" s="10"/>
-      <c r="M102" s="10"/>
-      <c r="N102" s="10"/>
-      <c r="O102" s="10"/>
-      <c r="P102" s="10"/>
-      <c r="Q102" s="10"/>
-      <c r="R102" s="10"/>
-      <c r="S102" s="10"/>
-      <c r="T102" s="10"/>
-      <c r="U102" s="10"/>
-      <c r="V102" s="10"/>
-      <c r="W102" s="10"/>
-      <c r="X102" s="10"/>
-      <c r="Y102" s="10"/>
-      <c r="Z102" s="10"/>
-      <c r="AA102" s="10"/>
+      <c r="L102" s="11"/>
+      <c r="M102" s="11"/>
+      <c r="N102" s="11"/>
+      <c r="O102" s="11"/>
+      <c r="P102" s="11"/>
+      <c r="Q102" s="11"/>
+      <c r="R102" s="11"/>
+      <c r="S102" s="11"/>
+      <c r="T102" s="11"/>
+      <c r="U102" s="11"/>
+      <c r="V102" s="11"/>
+      <c r="W102" s="11"/>
+      <c r="X102" s="11"/>
+      <c r="Y102" s="11"/>
+      <c r="Z102" s="11"/>
+      <c r="AA102" s="11"/>
     </row>
     <row r="103">
-      <c r="A103" s="7" t="s">
+      <c r="A103" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B103" s="7" t="s">
+      <c r="B103" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C103" s="8">
+      <c r="C103" s="9">
         <v>1.0</v>
       </c>
-      <c r="D103" s="8">
+      <c r="D103" s="9">
         <v>3.0</v>
       </c>
-      <c r="E103" s="7" t="s">
+      <c r="E103" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="F103" s="7" t="s">
+      <c r="F103" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="G103" s="9"/>
-      <c r="H103" s="8">
+      <c r="G103" s="10"/>
+      <c r="H103" s="9">
         <v>180.0</v>
       </c>
-      <c r="I103" s="8">
+      <c r="I103" s="9">
         <v>52.21</v>
       </c>
-      <c r="J103" s="8">
+      <c r="J103" s="9">
         <v>1.12</v>
       </c>
       <c r="K103" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Restio </v>
       </c>
-      <c r="L103" s="10"/>
-      <c r="M103" s="10"/>
-      <c r="N103" s="10"/>
-      <c r="O103" s="10"/>
-      <c r="P103" s="10"/>
-      <c r="Q103" s="10"/>
-      <c r="R103" s="10"/>
-      <c r="S103" s="10"/>
-      <c r="T103" s="10"/>
-      <c r="U103" s="10"/>
-      <c r="V103" s="10"/>
-      <c r="W103" s="10"/>
-      <c r="X103" s="10"/>
-      <c r="Y103" s="10"/>
-      <c r="Z103" s="10"/>
-      <c r="AA103" s="10"/>
+      <c r="L103" s="11"/>
+      <c r="M103" s="11"/>
+      <c r="N103" s="11"/>
+      <c r="O103" s="11"/>
+      <c r="P103" s="11"/>
+      <c r="Q103" s="11"/>
+      <c r="R103" s="11"/>
+      <c r="S103" s="11"/>
+      <c r="T103" s="11"/>
+      <c r="U103" s="11"/>
+      <c r="V103" s="11"/>
+      <c r="W103" s="11"/>
+      <c r="X103" s="11"/>
+      <c r="Y103" s="11"/>
+      <c r="Z103" s="11"/>
+      <c r="AA103" s="11"/>
     </row>
     <row r="104">
       <c r="A104" s="2" t="s">
@@ -22661,154 +22717,154 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="7" t="s">
+      <c r="A110" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B110" s="7" t="s">
+      <c r="B110" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C110" s="8">
+      <c r="C110" s="9">
         <v>4.0</v>
       </c>
-      <c r="D110" s="8">
+      <c r="D110" s="9">
         <v>1.0</v>
       </c>
-      <c r="E110" s="7" t="s">
+      <c r="E110" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="F110" s="7" t="s">
+      <c r="F110" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="G110" s="9"/>
-      <c r="H110" s="8">
+      <c r="G110" s="10"/>
+      <c r="H110" s="9">
         <v>150.0</v>
       </c>
-      <c r="I110" s="8">
+      <c r="I110" s="9">
         <v>1.22</v>
       </c>
-      <c r="J110" s="8">
+      <c r="J110" s="9">
         <v>6.07</v>
       </c>
       <c r="K110" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Poaceae </v>
       </c>
-      <c r="L110" s="10"/>
-      <c r="M110" s="10"/>
-      <c r="N110" s="10"/>
-      <c r="O110" s="10"/>
-      <c r="P110" s="10"/>
-      <c r="Q110" s="10"/>
-      <c r="R110" s="10"/>
-      <c r="S110" s="10"/>
-      <c r="T110" s="10"/>
-      <c r="U110" s="10"/>
-      <c r="V110" s="10"/>
-      <c r="W110" s="10"/>
-      <c r="X110" s="10"/>
-      <c r="Y110" s="10"/>
-      <c r="Z110" s="10"/>
-      <c r="AA110" s="10"/>
+      <c r="L110" s="11"/>
+      <c r="M110" s="11"/>
+      <c r="N110" s="11"/>
+      <c r="O110" s="11"/>
+      <c r="P110" s="11"/>
+      <c r="Q110" s="11"/>
+      <c r="R110" s="11"/>
+      <c r="S110" s="11"/>
+      <c r="T110" s="11"/>
+      <c r="U110" s="11"/>
+      <c r="V110" s="11"/>
+      <c r="W110" s="11"/>
+      <c r="X110" s="11"/>
+      <c r="Y110" s="11"/>
+      <c r="Z110" s="11"/>
+      <c r="AA110" s="11"/>
     </row>
     <row r="111">
-      <c r="A111" s="7" t="s">
+      <c r="A111" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B111" s="7" t="s">
+      <c r="B111" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C111" s="8">
+      <c r="C111" s="9">
         <v>4.0</v>
       </c>
-      <c r="D111" s="8">
+      <c r="D111" s="9">
         <v>2.0</v>
       </c>
-      <c r="E111" s="7" t="s">
+      <c r="E111" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="F111" s="7" t="s">
+      <c r="F111" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="G111" s="9"/>
-      <c r="H111" s="8">
+      <c r="G111" s="10"/>
+      <c r="H111" s="9">
         <v>890.0</v>
       </c>
-      <c r="I111" s="8">
+      <c r="I111" s="9">
         <v>1.33</v>
       </c>
-      <c r="J111" s="8">
+      <c r="J111" s="9">
         <v>6.88</v>
       </c>
       <c r="K111" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Poaceae </v>
       </c>
-      <c r="L111" s="10"/>
-      <c r="M111" s="10"/>
-      <c r="N111" s="10"/>
-      <c r="O111" s="10"/>
-      <c r="P111" s="10"/>
-      <c r="Q111" s="10"/>
-      <c r="R111" s="10"/>
-      <c r="S111" s="10"/>
-      <c r="T111" s="10"/>
-      <c r="U111" s="10"/>
-      <c r="V111" s="10"/>
-      <c r="W111" s="10"/>
-      <c r="X111" s="10"/>
-      <c r="Y111" s="10"/>
-      <c r="Z111" s="10"/>
-      <c r="AA111" s="10"/>
+      <c r="L111" s="11"/>
+      <c r="M111" s="11"/>
+      <c r="N111" s="11"/>
+      <c r="O111" s="11"/>
+      <c r="P111" s="11"/>
+      <c r="Q111" s="11"/>
+      <c r="R111" s="11"/>
+      <c r="S111" s="11"/>
+      <c r="T111" s="11"/>
+      <c r="U111" s="11"/>
+      <c r="V111" s="11"/>
+      <c r="W111" s="11"/>
+      <c r="X111" s="11"/>
+      <c r="Y111" s="11"/>
+      <c r="Z111" s="11"/>
+      <c r="AA111" s="11"/>
     </row>
     <row r="112">
-      <c r="A112" s="7" t="s">
+      <c r="A112" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B112" s="7" t="s">
+      <c r="B112" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C112" s="8">
+      <c r="C112" s="9">
         <v>4.0</v>
       </c>
-      <c r="D112" s="8">
+      <c r="D112" s="9">
         <v>3.0</v>
       </c>
-      <c r="E112" s="7" t="s">
+      <c r="E112" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="F112" s="7" t="s">
+      <c r="F112" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="G112" s="9"/>
-      <c r="H112" s="8">
+      <c r="G112" s="10"/>
+      <c r="H112" s="9">
         <v>131.0</v>
       </c>
-      <c r="I112" s="8">
+      <c r="I112" s="9">
         <v>76.0</v>
       </c>
-      <c r="J112" s="8">
+      <c r="J112" s="9">
         <v>6.31</v>
       </c>
       <c r="K112" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Poaceae </v>
       </c>
-      <c r="L112" s="10"/>
-      <c r="M112" s="10"/>
-      <c r="N112" s="10"/>
-      <c r="O112" s="10"/>
-      <c r="P112" s="10"/>
-      <c r="Q112" s="10"/>
-      <c r="R112" s="10"/>
-      <c r="S112" s="10"/>
-      <c r="T112" s="10"/>
-      <c r="U112" s="10"/>
-      <c r="V112" s="10"/>
-      <c r="W112" s="10"/>
-      <c r="X112" s="10"/>
-      <c r="Y112" s="10"/>
-      <c r="Z112" s="10"/>
-      <c r="AA112" s="10"/>
+      <c r="L112" s="11"/>
+      <c r="M112" s="11"/>
+      <c r="N112" s="11"/>
+      <c r="O112" s="11"/>
+      <c r="P112" s="11"/>
+      <c r="Q112" s="11"/>
+      <c r="R112" s="11"/>
+      <c r="S112" s="11"/>
+      <c r="T112" s="11"/>
+      <c r="U112" s="11"/>
+      <c r="V112" s="11"/>
+      <c r="W112" s="11"/>
+      <c r="X112" s="11"/>
+      <c r="Y112" s="11"/>
+      <c r="Z112" s="11"/>
+      <c r="AA112" s="11"/>
     </row>
     <row r="113">
       <c r="A113" s="2" t="s">
@@ -23243,154 +23299,154 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="7" t="s">
+      <c r="A125" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B125" s="7" t="s">
+      <c r="B125" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C125" s="8">
+      <c r="C125" s="9">
         <v>4.0</v>
       </c>
-      <c r="D125" s="8">
+      <c r="D125" s="9">
         <v>1.0</v>
       </c>
-      <c r="E125" s="7" t="s">
+      <c r="E125" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="F125" s="7" t="s">
+      <c r="F125" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G125" s="9"/>
-      <c r="H125" s="8">
+      <c r="G125" s="10"/>
+      <c r="H125" s="9">
         <v>950.0</v>
       </c>
-      <c r="I125" s="8">
+      <c r="I125" s="9">
         <v>3.55</v>
       </c>
-      <c r="J125" s="8">
+      <c r="J125" s="9">
         <v>1.98</v>
       </c>
       <c r="K125" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Bruniaceae </v>
       </c>
-      <c r="L125" s="10"/>
-      <c r="M125" s="10"/>
-      <c r="N125" s="10"/>
-      <c r="O125" s="10"/>
-      <c r="P125" s="10"/>
-      <c r="Q125" s="10"/>
-      <c r="R125" s="10"/>
-      <c r="S125" s="10"/>
-      <c r="T125" s="10"/>
-      <c r="U125" s="10"/>
-      <c r="V125" s="10"/>
-      <c r="W125" s="10"/>
-      <c r="X125" s="10"/>
-      <c r="Y125" s="10"/>
-      <c r="Z125" s="10"/>
-      <c r="AA125" s="10"/>
+      <c r="L125" s="11"/>
+      <c r="M125" s="11"/>
+      <c r="N125" s="11"/>
+      <c r="O125" s="11"/>
+      <c r="P125" s="11"/>
+      <c r="Q125" s="11"/>
+      <c r="R125" s="11"/>
+      <c r="S125" s="11"/>
+      <c r="T125" s="11"/>
+      <c r="U125" s="11"/>
+      <c r="V125" s="11"/>
+      <c r="W125" s="11"/>
+      <c r="X125" s="11"/>
+      <c r="Y125" s="11"/>
+      <c r="Z125" s="11"/>
+      <c r="AA125" s="11"/>
     </row>
     <row r="126">
-      <c r="A126" s="7" t="s">
+      <c r="A126" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B126" s="7" t="s">
+      <c r="B126" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C126" s="8">
+      <c r="C126" s="9">
         <v>4.0</v>
       </c>
-      <c r="D126" s="8">
+      <c r="D126" s="9">
         <v>2.0</v>
       </c>
-      <c r="E126" s="7" t="s">
+      <c r="E126" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="F126" s="7" t="s">
+      <c r="F126" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G126" s="9"/>
-      <c r="H126" s="8">
+      <c r="G126" s="10"/>
+      <c r="H126" s="9">
         <v>785.0</v>
       </c>
-      <c r="I126" s="8">
+      <c r="I126" s="9">
         <v>3.53</v>
       </c>
-      <c r="J126" s="8">
+      <c r="J126" s="9">
         <v>0.5</v>
       </c>
       <c r="K126" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Bruniaceae </v>
       </c>
-      <c r="L126" s="10"/>
-      <c r="M126" s="10"/>
-      <c r="N126" s="10"/>
-      <c r="O126" s="10"/>
-      <c r="P126" s="10"/>
-      <c r="Q126" s="10"/>
-      <c r="R126" s="10"/>
-      <c r="S126" s="10"/>
-      <c r="T126" s="10"/>
-      <c r="U126" s="10"/>
-      <c r="V126" s="10"/>
-      <c r="W126" s="10"/>
-      <c r="X126" s="10"/>
-      <c r="Y126" s="10"/>
-      <c r="Z126" s="10"/>
-      <c r="AA126" s="10"/>
+      <c r="L126" s="11"/>
+      <c r="M126" s="11"/>
+      <c r="N126" s="11"/>
+      <c r="O126" s="11"/>
+      <c r="P126" s="11"/>
+      <c r="Q126" s="11"/>
+      <c r="R126" s="11"/>
+      <c r="S126" s="11"/>
+      <c r="T126" s="11"/>
+      <c r="U126" s="11"/>
+      <c r="V126" s="11"/>
+      <c r="W126" s="11"/>
+      <c r="X126" s="11"/>
+      <c r="Y126" s="11"/>
+      <c r="Z126" s="11"/>
+      <c r="AA126" s="11"/>
     </row>
     <row r="127">
-      <c r="A127" s="7" t="s">
+      <c r="A127" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B127" s="7" t="s">
+      <c r="B127" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C127" s="8">
+      <c r="C127" s="9">
         <v>4.0</v>
       </c>
-      <c r="D127" s="8">
+      <c r="D127" s="9">
         <v>3.0</v>
       </c>
-      <c r="E127" s="7" t="s">
+      <c r="E127" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="F127" s="7" t="s">
+      <c r="F127" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G127" s="9"/>
-      <c r="H127" s="8">
+      <c r="G127" s="10"/>
+      <c r="H127" s="9">
         <v>1000.0</v>
       </c>
-      <c r="I127" s="8">
+      <c r="I127" s="9">
         <v>3.94</v>
       </c>
-      <c r="J127" s="8">
+      <c r="J127" s="9">
         <v>2.23</v>
       </c>
       <c r="K127" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Bruniaceae </v>
       </c>
-      <c r="L127" s="10"/>
-      <c r="M127" s="10"/>
-      <c r="N127" s="10"/>
-      <c r="O127" s="10"/>
-      <c r="P127" s="10"/>
-      <c r="Q127" s="10"/>
-      <c r="R127" s="10"/>
-      <c r="S127" s="10"/>
-      <c r="T127" s="10"/>
-      <c r="U127" s="10"/>
-      <c r="V127" s="10"/>
-      <c r="W127" s="10"/>
-      <c r="X127" s="10"/>
-      <c r="Y127" s="10"/>
-      <c r="Z127" s="10"/>
-      <c r="AA127" s="10"/>
+      <c r="L127" s="11"/>
+      <c r="M127" s="11"/>
+      <c r="N127" s="11"/>
+      <c r="O127" s="11"/>
+      <c r="P127" s="11"/>
+      <c r="Q127" s="11"/>
+      <c r="R127" s="11"/>
+      <c r="S127" s="11"/>
+      <c r="T127" s="11"/>
+      <c r="U127" s="11"/>
+      <c r="V127" s="11"/>
+      <c r="W127" s="11"/>
+      <c r="X127" s="11"/>
+      <c r="Y127" s="11"/>
+      <c r="Z127" s="11"/>
+      <c r="AA127" s="11"/>
     </row>
     <row r="128">
       <c r="A128" s="2" t="s">
@@ -23411,7 +23467,7 @@
       <c r="F128" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G128" s="4"/>
+      <c r="G128" s="7"/>
       <c r="H128" s="3">
         <v>133.0</v>
       </c>
@@ -23445,7 +23501,7 @@
       <c r="F129" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G129" s="4"/>
+      <c r="G129" s="7"/>
       <c r="H129" s="3">
         <v>140.0</v>
       </c>
@@ -23479,7 +23535,7 @@
       <c r="F130" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G130" s="4"/>
+      <c r="G130" s="7"/>
       <c r="H130" s="3">
         <v>125.0</v>
       </c>
@@ -23513,7 +23569,7 @@
       <c r="F131" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G131" s="4"/>
+      <c r="G131" s="7"/>
       <c r="H131" s="3">
         <v>122.0</v>
       </c>
@@ -23547,7 +23603,7 @@
       <c r="F132" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G132" s="4"/>
+      <c r="G132" s="7"/>
       <c r="H132" s="3">
         <v>107.0</v>
       </c>
@@ -23581,7 +23637,7 @@
       <c r="F133" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G133" s="4"/>
+      <c r="G133" s="7"/>
       <c r="H133" s="3">
         <v>120.0</v>
       </c>
@@ -23831,7 +23887,7 @@
       <c r="F140" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G140" s="4"/>
+      <c r="G140" s="7"/>
       <c r="H140" s="3">
         <v>110.0</v>
       </c>
@@ -23865,7 +23921,7 @@
       <c r="F141" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G141" s="4"/>
+      <c r="G141" s="7"/>
       <c r="H141" s="3">
         <v>65.0</v>
       </c>
@@ -23899,7 +23955,7 @@
       <c r="F142" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G142" s="4"/>
+      <c r="G142" s="7"/>
       <c r="H142" s="3">
         <v>122.0</v>
       </c>
@@ -24131,154 +24187,154 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="7" t="s">
+      <c r="A149" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B149" s="7" t="s">
+      <c r="B149" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C149" s="8">
+      <c r="C149" s="9">
         <v>5.0</v>
       </c>
-      <c r="D149" s="8">
+      <c r="D149" s="9">
         <v>1.0</v>
       </c>
-      <c r="E149" s="7" t="s">
+      <c r="E149" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="F149" s="7" t="s">
+      <c r="F149" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="G149" s="9"/>
-      <c r="H149" s="8">
+      <c r="G149" s="10"/>
+      <c r="H149" s="9">
         <v>39.6</v>
       </c>
-      <c r="I149" s="8">
+      <c r="I149" s="9">
         <v>18.2</v>
       </c>
-      <c r="J149" s="8">
+      <c r="J149" s="9">
         <v>0.44</v>
       </c>
       <c r="K149" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Restio </v>
       </c>
-      <c r="L149" s="10"/>
-      <c r="M149" s="10"/>
-      <c r="N149" s="10"/>
-      <c r="O149" s="10"/>
-      <c r="P149" s="10"/>
-      <c r="Q149" s="10"/>
-      <c r="R149" s="10"/>
-      <c r="S149" s="10"/>
-      <c r="T149" s="10"/>
-      <c r="U149" s="10"/>
-      <c r="V149" s="10"/>
-      <c r="W149" s="10"/>
-      <c r="X149" s="10"/>
-      <c r="Y149" s="10"/>
-      <c r="Z149" s="10"/>
-      <c r="AA149" s="10"/>
+      <c r="L149" s="11"/>
+      <c r="M149" s="11"/>
+      <c r="N149" s="11"/>
+      <c r="O149" s="11"/>
+      <c r="P149" s="11"/>
+      <c r="Q149" s="11"/>
+      <c r="R149" s="11"/>
+      <c r="S149" s="11"/>
+      <c r="T149" s="11"/>
+      <c r="U149" s="11"/>
+      <c r="V149" s="11"/>
+      <c r="W149" s="11"/>
+      <c r="X149" s="11"/>
+      <c r="Y149" s="11"/>
+      <c r="Z149" s="11"/>
+      <c r="AA149" s="11"/>
     </row>
     <row r="150">
-      <c r="A150" s="7" t="s">
+      <c r="A150" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B150" s="7" t="s">
+      <c r="B150" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C150" s="8">
+      <c r="C150" s="9">
         <v>5.0</v>
       </c>
-      <c r="D150" s="8">
+      <c r="D150" s="9">
         <v>2.0</v>
       </c>
-      <c r="E150" s="7" t="s">
+      <c r="E150" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="F150" s="7" t="s">
+      <c r="F150" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="G150" s="9"/>
-      <c r="H150" s="8">
+      <c r="G150" s="10"/>
+      <c r="H150" s="9">
         <v>42.0</v>
       </c>
-      <c r="I150" s="8">
+      <c r="I150" s="9">
         <v>21.69</v>
       </c>
-      <c r="J150" s="8">
+      <c r="J150" s="9">
         <v>0.57</v>
       </c>
       <c r="K150" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Restio </v>
       </c>
-      <c r="L150" s="10"/>
-      <c r="M150" s="10"/>
-      <c r="N150" s="10"/>
-      <c r="O150" s="10"/>
-      <c r="P150" s="10"/>
-      <c r="Q150" s="10"/>
-      <c r="R150" s="10"/>
-      <c r="S150" s="10"/>
-      <c r="T150" s="10"/>
-      <c r="U150" s="10"/>
-      <c r="V150" s="10"/>
-      <c r="W150" s="10"/>
-      <c r="X150" s="10"/>
-      <c r="Y150" s="10"/>
-      <c r="Z150" s="10"/>
-      <c r="AA150" s="10"/>
+      <c r="L150" s="11"/>
+      <c r="M150" s="11"/>
+      <c r="N150" s="11"/>
+      <c r="O150" s="11"/>
+      <c r="P150" s="11"/>
+      <c r="Q150" s="11"/>
+      <c r="R150" s="11"/>
+      <c r="S150" s="11"/>
+      <c r="T150" s="11"/>
+      <c r="U150" s="11"/>
+      <c r="V150" s="11"/>
+      <c r="W150" s="11"/>
+      <c r="X150" s="11"/>
+      <c r="Y150" s="11"/>
+      <c r="Z150" s="11"/>
+      <c r="AA150" s="11"/>
     </row>
     <row r="151">
-      <c r="A151" s="7" t="s">
+      <c r="A151" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B151" s="7" t="s">
+      <c r="B151" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C151" s="8">
+      <c r="C151" s="9">
         <v>5.0</v>
       </c>
-      <c r="D151" s="8">
+      <c r="D151" s="9">
         <v>3.0</v>
       </c>
-      <c r="E151" s="7" t="s">
+      <c r="E151" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="F151" s="7" t="s">
+      <c r="F151" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="G151" s="9"/>
-      <c r="H151" s="8">
+      <c r="G151" s="10"/>
+      <c r="H151" s="9">
         <v>54.0</v>
       </c>
-      <c r="I151" s="8">
+      <c r="I151" s="9">
         <v>27.76</v>
       </c>
-      <c r="J151" s="8">
+      <c r="J151" s="9">
         <v>0.52</v>
       </c>
       <c r="K151" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Restio </v>
       </c>
-      <c r="L151" s="10"/>
-      <c r="M151" s="10"/>
-      <c r="N151" s="10"/>
-      <c r="O151" s="10"/>
-      <c r="P151" s="10"/>
-      <c r="Q151" s="10"/>
-      <c r="R151" s="10"/>
-      <c r="S151" s="10"/>
-      <c r="T151" s="10"/>
-      <c r="U151" s="10"/>
-      <c r="V151" s="10"/>
-      <c r="W151" s="10"/>
-      <c r="X151" s="10"/>
-      <c r="Y151" s="10"/>
-      <c r="Z151" s="10"/>
-      <c r="AA151" s="10"/>
+      <c r="L151" s="11"/>
+      <c r="M151" s="11"/>
+      <c r="N151" s="11"/>
+      <c r="O151" s="11"/>
+      <c r="P151" s="11"/>
+      <c r="Q151" s="11"/>
+      <c r="R151" s="11"/>
+      <c r="S151" s="11"/>
+      <c r="T151" s="11"/>
+      <c r="U151" s="11"/>
+      <c r="V151" s="11"/>
+      <c r="W151" s="11"/>
+      <c r="X151" s="11"/>
+      <c r="Y151" s="11"/>
+      <c r="Z151" s="11"/>
+      <c r="AA151" s="11"/>
     </row>
     <row r="152">
       <c r="A152" s="2" t="s">
@@ -24407,7 +24463,7 @@
       <c r="F155" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G155" s="4"/>
+      <c r="G155" s="7"/>
       <c r="H155" s="3">
         <v>200.0</v>
       </c>
@@ -24441,7 +24497,7 @@
       <c r="F156" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G156" s="4"/>
+      <c r="G156" s="7"/>
       <c r="H156" s="3">
         <v>230.0</v>
       </c>
@@ -24475,7 +24531,7 @@
       <c r="F157" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G157" s="4"/>
+      <c r="G157" s="7"/>
       <c r="H157" s="3">
         <v>190.0</v>
       </c>
@@ -24509,7 +24565,7 @@
       <c r="F158" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="G158" s="4"/>
+      <c r="G158" s="7"/>
       <c r="H158" s="3">
         <v>60.0</v>
       </c>
@@ -24543,7 +24599,7 @@
       <c r="F159" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="G159" s="4"/>
+      <c r="G159" s="7"/>
       <c r="H159" s="3">
         <v>59.8</v>
       </c>
@@ -24577,7 +24633,7 @@
       <c r="F160" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="G160" s="4"/>
+      <c r="G160" s="7"/>
       <c r="H160" s="3">
         <v>70.0</v>
       </c>
@@ -25025,148 +25081,148 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" s="7" t="s">
+      <c r="A173" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B173" s="7" t="s">
+      <c r="B173" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C173" s="8">
+      <c r="C173" s="9">
         <v>3.0</v>
       </c>
-      <c r="D173" s="8">
+      <c r="D173" s="9">
         <v>1.0</v>
       </c>
-      <c r="E173" s="7" t="s">
+      <c r="E173" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="F173" s="11" t="s">
+      <c r="F173" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="G173" s="11" t="s">
+      <c r="G173" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="H173" s="8">
+      <c r="H173" s="9">
         <v>26.0</v>
       </c>
-      <c r="I173" s="7"/>
-      <c r="J173" s="7"/>
+      <c r="I173" s="8"/>
+      <c r="J173" s="8"/>
       <c r="K173" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Trifolium angustifolium</v>
       </c>
-      <c r="L173" s="10"/>
-      <c r="M173" s="10"/>
-      <c r="N173" s="10"/>
-      <c r="O173" s="10"/>
-      <c r="P173" s="10"/>
-      <c r="Q173" s="10"/>
-      <c r="R173" s="10"/>
-      <c r="S173" s="10"/>
-      <c r="T173" s="10"/>
-      <c r="U173" s="10"/>
-      <c r="V173" s="10"/>
-      <c r="W173" s="10"/>
-      <c r="X173" s="10"/>
-      <c r="Y173" s="10"/>
-      <c r="Z173" s="10"/>
-      <c r="AA173" s="10"/>
+      <c r="L173" s="11"/>
+      <c r="M173" s="11"/>
+      <c r="N173" s="11"/>
+      <c r="O173" s="11"/>
+      <c r="P173" s="11"/>
+      <c r="Q173" s="11"/>
+      <c r="R173" s="11"/>
+      <c r="S173" s="11"/>
+      <c r="T173" s="11"/>
+      <c r="U173" s="11"/>
+      <c r="V173" s="11"/>
+      <c r="W173" s="11"/>
+      <c r="X173" s="11"/>
+      <c r="Y173" s="11"/>
+      <c r="Z173" s="11"/>
+      <c r="AA173" s="11"/>
     </row>
     <row r="174">
-      <c r="A174" s="7" t="s">
+      <c r="A174" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B174" s="7" t="s">
+      <c r="B174" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C174" s="8">
+      <c r="C174" s="9">
         <v>3.0</v>
       </c>
-      <c r="D174" s="8">
+      <c r="D174" s="9">
         <v>2.0</v>
       </c>
-      <c r="E174" s="7" t="s">
+      <c r="E174" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="F174" s="11" t="s">
+      <c r="F174" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="G174" s="11" t="s">
+      <c r="G174" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="H174" s="8">
+      <c r="H174" s="9">
         <v>27.0</v>
       </c>
-      <c r="I174" s="7"/>
-      <c r="J174" s="7"/>
+      <c r="I174" s="8"/>
+      <c r="J174" s="8"/>
       <c r="K174" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Trifolium angustifolium</v>
       </c>
-      <c r="L174" s="10"/>
-      <c r="M174" s="10"/>
-      <c r="N174" s="10"/>
-      <c r="O174" s="10"/>
-      <c r="P174" s="10"/>
-      <c r="Q174" s="10"/>
-      <c r="R174" s="10"/>
-      <c r="S174" s="10"/>
-      <c r="T174" s="10"/>
-      <c r="U174" s="10"/>
-      <c r="V174" s="10"/>
-      <c r="W174" s="10"/>
-      <c r="X174" s="10"/>
-      <c r="Y174" s="10"/>
-      <c r="Z174" s="10"/>
-      <c r="AA174" s="10"/>
+      <c r="L174" s="11"/>
+      <c r="M174" s="11"/>
+      <c r="N174" s="11"/>
+      <c r="O174" s="11"/>
+      <c r="P174" s="11"/>
+      <c r="Q174" s="11"/>
+      <c r="R174" s="11"/>
+      <c r="S174" s="11"/>
+      <c r="T174" s="11"/>
+      <c r="U174" s="11"/>
+      <c r="V174" s="11"/>
+      <c r="W174" s="11"/>
+      <c r="X174" s="11"/>
+      <c r="Y174" s="11"/>
+      <c r="Z174" s="11"/>
+      <c r="AA174" s="11"/>
     </row>
     <row r="175">
-      <c r="A175" s="7" t="s">
+      <c r="A175" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B175" s="7" t="s">
+      <c r="B175" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C175" s="8">
+      <c r="C175" s="9">
         <v>3.0</v>
       </c>
-      <c r="D175" s="8">
+      <c r="D175" s="9">
         <v>3.0</v>
       </c>
-      <c r="E175" s="7" t="s">
+      <c r="E175" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="F175" s="11" t="s">
+      <c r="F175" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="G175" s="11" t="s">
+      <c r="G175" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="H175" s="8">
+      <c r="H175" s="9">
         <v>18.0</v>
       </c>
-      <c r="I175" s="7"/>
-      <c r="J175" s="7"/>
+      <c r="I175" s="8"/>
+      <c r="J175" s="8"/>
       <c r="K175" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Trifolium angustifolium</v>
       </c>
-      <c r="L175" s="10"/>
-      <c r="M175" s="10"/>
-      <c r="N175" s="10"/>
-      <c r="O175" s="10"/>
-      <c r="P175" s="10"/>
-      <c r="Q175" s="10"/>
-      <c r="R175" s="10"/>
-      <c r="S175" s="10"/>
-      <c r="T175" s="10"/>
-      <c r="U175" s="10"/>
-      <c r="V175" s="10"/>
-      <c r="W175" s="10"/>
-      <c r="X175" s="10"/>
-      <c r="Y175" s="10"/>
-      <c r="Z175" s="10"/>
-      <c r="AA175" s="10"/>
+      <c r="L175" s="11"/>
+      <c r="M175" s="11"/>
+      <c r="N175" s="11"/>
+      <c r="O175" s="11"/>
+      <c r="P175" s="11"/>
+      <c r="Q175" s="11"/>
+      <c r="R175" s="11"/>
+      <c r="S175" s="11"/>
+      <c r="T175" s="11"/>
+      <c r="U175" s="11"/>
+      <c r="V175" s="11"/>
+      <c r="W175" s="11"/>
+      <c r="X175" s="11"/>
+      <c r="Y175" s="11"/>
+      <c r="Z175" s="11"/>
+      <c r="AA175" s="11"/>
     </row>
     <row r="176">
       <c r="A176" s="2" t="s">
@@ -25295,7 +25351,7 @@
       <c r="F179" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="G179" s="4"/>
+      <c r="G179" s="7"/>
       <c r="H179" s="3">
         <v>62.0</v>
       </c>
@@ -25329,7 +25385,7 @@
       <c r="F180" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="G180" s="4"/>
+      <c r="G180" s="7"/>
       <c r="H180" s="3">
         <v>47.0</v>
       </c>
@@ -25363,7 +25419,7 @@
       <c r="F181" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="G181" s="4"/>
+      <c r="G181" s="7"/>
       <c r="H181" s="3">
         <v>48.0</v>
       </c>
@@ -25487,154 +25543,154 @@
       </c>
     </row>
     <row r="185">
-      <c r="A185" s="7" t="s">
+      <c r="A185" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B185" s="7" t="s">
+      <c r="B185" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C185" s="8">
+      <c r="C185" s="9">
         <v>2.0</v>
       </c>
-      <c r="D185" s="8">
+      <c r="D185" s="9">
         <v>1.0</v>
       </c>
-      <c r="E185" s="7" t="s">
+      <c r="E185" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="F185" s="12" t="s">
+      <c r="F185" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="G185" s="9"/>
-      <c r="H185" s="8">
+      <c r="G185" s="10"/>
+      <c r="H185" s="9">
         <v>140.0</v>
       </c>
-      <c r="I185" s="8">
+      <c r="I185" s="9">
         <v>890.0</v>
       </c>
-      <c r="J185" s="8">
+      <c r="J185" s="9">
         <v>1.14</v>
       </c>
       <c r="K185" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Poaceae </v>
       </c>
-      <c r="L185" s="10"/>
-      <c r="M185" s="10"/>
-      <c r="N185" s="10"/>
-      <c r="O185" s="10"/>
-      <c r="P185" s="10"/>
-      <c r="Q185" s="10"/>
-      <c r="R185" s="10"/>
-      <c r="S185" s="10"/>
-      <c r="T185" s="10"/>
-      <c r="U185" s="10"/>
-      <c r="V185" s="10"/>
-      <c r="W185" s="10"/>
-      <c r="X185" s="10"/>
-      <c r="Y185" s="10"/>
-      <c r="Z185" s="10"/>
-      <c r="AA185" s="10"/>
+      <c r="L185" s="11"/>
+      <c r="M185" s="11"/>
+      <c r="N185" s="11"/>
+      <c r="O185" s="11"/>
+      <c r="P185" s="11"/>
+      <c r="Q185" s="11"/>
+      <c r="R185" s="11"/>
+      <c r="S185" s="11"/>
+      <c r="T185" s="11"/>
+      <c r="U185" s="11"/>
+      <c r="V185" s="11"/>
+      <c r="W185" s="11"/>
+      <c r="X185" s="11"/>
+      <c r="Y185" s="11"/>
+      <c r="Z185" s="11"/>
+      <c r="AA185" s="11"/>
     </row>
     <row r="186">
-      <c r="A186" s="7" t="s">
+      <c r="A186" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B186" s="7" t="s">
+      <c r="B186" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C186" s="8">
+      <c r="C186" s="9">
         <v>2.0</v>
       </c>
-      <c r="D186" s="8">
+      <c r="D186" s="9">
         <v>2.0</v>
       </c>
-      <c r="E186" s="7" t="s">
+      <c r="E186" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="F186" s="12" t="s">
+      <c r="F186" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="G186" s="9"/>
-      <c r="H186" s="8">
+      <c r="G186" s="10"/>
+      <c r="H186" s="9">
         <v>160.0</v>
       </c>
-      <c r="I186" s="8">
+      <c r="I186" s="9">
         <v>920.0</v>
       </c>
-      <c r="J186" s="8">
+      <c r="J186" s="9">
         <v>2.51</v>
       </c>
       <c r="K186" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Poaceae </v>
       </c>
-      <c r="L186" s="10"/>
-      <c r="M186" s="10"/>
-      <c r="N186" s="10"/>
-      <c r="O186" s="10"/>
-      <c r="P186" s="10"/>
-      <c r="Q186" s="10"/>
-      <c r="R186" s="10"/>
-      <c r="S186" s="10"/>
-      <c r="T186" s="10"/>
-      <c r="U186" s="10"/>
-      <c r="V186" s="10"/>
-      <c r="W186" s="10"/>
-      <c r="X186" s="10"/>
-      <c r="Y186" s="10"/>
-      <c r="Z186" s="10"/>
-      <c r="AA186" s="10"/>
+      <c r="L186" s="11"/>
+      <c r="M186" s="11"/>
+      <c r="N186" s="11"/>
+      <c r="O186" s="11"/>
+      <c r="P186" s="11"/>
+      <c r="Q186" s="11"/>
+      <c r="R186" s="11"/>
+      <c r="S186" s="11"/>
+      <c r="T186" s="11"/>
+      <c r="U186" s="11"/>
+      <c r="V186" s="11"/>
+      <c r="W186" s="11"/>
+      <c r="X186" s="11"/>
+      <c r="Y186" s="11"/>
+      <c r="Z186" s="11"/>
+      <c r="AA186" s="11"/>
     </row>
     <row r="187">
-      <c r="A187" s="7" t="s">
+      <c r="A187" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B187" s="7" t="s">
+      <c r="B187" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C187" s="8">
+      <c r="C187" s="9">
         <v>2.0</v>
       </c>
-      <c r="D187" s="8">
+      <c r="D187" s="9">
         <v>3.0</v>
       </c>
-      <c r="E187" s="7" t="s">
+      <c r="E187" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="F187" s="12" t="s">
+      <c r="F187" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="G187" s="9"/>
-      <c r="H187" s="8">
+      <c r="G187" s="10"/>
+      <c r="H187" s="9">
         <v>240.0</v>
       </c>
-      <c r="I187" s="8">
+      <c r="I187" s="9">
         <v>2000.0</v>
       </c>
-      <c r="J187" s="8">
+      <c r="J187" s="9">
         <v>3.11</v>
       </c>
       <c r="K187" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Poaceae </v>
       </c>
-      <c r="L187" s="10"/>
-      <c r="M187" s="10"/>
-      <c r="N187" s="10"/>
-      <c r="O187" s="10"/>
-      <c r="P187" s="10"/>
-      <c r="Q187" s="10"/>
-      <c r="R187" s="10"/>
-      <c r="S187" s="10"/>
-      <c r="T187" s="10"/>
-      <c r="U187" s="10"/>
-      <c r="V187" s="10"/>
-      <c r="W187" s="10"/>
-      <c r="X187" s="10"/>
-      <c r="Y187" s="10"/>
-      <c r="Z187" s="10"/>
-      <c r="AA187" s="10"/>
+      <c r="L187" s="11"/>
+      <c r="M187" s="11"/>
+      <c r="N187" s="11"/>
+      <c r="O187" s="11"/>
+      <c r="P187" s="11"/>
+      <c r="Q187" s="11"/>
+      <c r="R187" s="11"/>
+      <c r="S187" s="11"/>
+      <c r="T187" s="11"/>
+      <c r="U187" s="11"/>
+      <c r="V187" s="11"/>
+      <c r="W187" s="11"/>
+      <c r="X187" s="11"/>
+      <c r="Y187" s="11"/>
+      <c r="Z187" s="11"/>
+      <c r="AA187" s="11"/>
     </row>
     <row r="188">
       <c r="A188" s="2" t="s">
@@ -25979,7 +26035,7 @@
       <c r="F197" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G197" s="4"/>
+      <c r="G197" s="7"/>
       <c r="H197" s="3">
         <v>95.0</v>
       </c>
@@ -26013,7 +26069,7 @@
       <c r="F198" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G198" s="4"/>
+      <c r="G198" s="7"/>
       <c r="H198" s="3">
         <v>120.0</v>
       </c>
@@ -26047,7 +26103,7 @@
       <c r="F199" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G199" s="4"/>
+      <c r="G199" s="7"/>
       <c r="H199" s="3">
         <v>98.0</v>
       </c>
@@ -26189,7 +26245,7 @@
       <c r="F203" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G203" s="4"/>
+      <c r="G203" s="7"/>
       <c r="H203" s="3">
         <v>60.0</v>
       </c>
@@ -26223,7 +26279,7 @@
       <c r="F204" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G204" s="4"/>
+      <c r="G204" s="7"/>
       <c r="H204" s="3">
         <v>55.0</v>
       </c>
@@ -26257,7 +26313,7 @@
       <c r="F205" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G205" s="4"/>
+      <c r="G205" s="7"/>
       <c r="H205" s="3">
         <v>58.0</v>
       </c>
@@ -26507,7 +26563,7 @@
       <c r="F212" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G212" s="4"/>
+      <c r="G212" s="7"/>
       <c r="H212" s="3">
         <v>45.0</v>
       </c>
@@ -26541,7 +26597,7 @@
       <c r="F213" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G213" s="4"/>
+      <c r="G213" s="7"/>
       <c r="H213" s="3">
         <v>35.0</v>
       </c>
@@ -26575,7 +26631,7 @@
       <c r="F214" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G214" s="4"/>
+      <c r="G214" s="7"/>
       <c r="H214" s="3">
         <v>50.0</v>
       </c>
@@ -26717,7 +26773,7 @@
       <c r="F218" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G218" s="4"/>
+      <c r="G218" s="7"/>
       <c r="H218" s="3">
         <v>70.0</v>
       </c>
@@ -26751,7 +26807,7 @@
       <c r="F219" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G219" s="4"/>
+      <c r="G219" s="7"/>
       <c r="H219" s="3">
         <v>78.0</v>
       </c>
@@ -26785,7 +26841,7 @@
       <c r="F220" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G220" s="4"/>
+      <c r="G220" s="7"/>
       <c r="H220" s="3">
         <v>90.0</v>
       </c>
@@ -26819,7 +26875,7 @@
       <c r="F221" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G221" s="4"/>
+      <c r="G221" s="7"/>
       <c r="H221" s="3">
         <v>110.0</v>
       </c>
@@ -26853,7 +26909,7 @@
       <c r="F222" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G222" s="4"/>
+      <c r="G222" s="7"/>
       <c r="H222" s="3">
         <v>150.0</v>
       </c>
@@ -26887,7 +26943,7 @@
       <c r="F223" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G223" s="4"/>
+      <c r="G223" s="7"/>
       <c r="H223" s="3">
         <v>110.0</v>
       </c>
@@ -26921,7 +26977,7 @@
       <c r="F224" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="G224" s="4"/>
+      <c r="G224" s="7"/>
       <c r="H224" s="3">
         <v>120.0</v>
       </c>
@@ -26955,7 +27011,7 @@
       <c r="F225" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="G225" s="4"/>
+      <c r="G225" s="7"/>
       <c r="H225" s="3">
         <v>150.0</v>
       </c>
@@ -26989,7 +27045,7 @@
       <c r="F226" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="G226" s="4"/>
+      <c r="G226" s="7"/>
       <c r="H226" s="3">
         <v>120.0</v>
       </c>
@@ -27221,154 +27277,154 @@
       </c>
     </row>
     <row r="233">
-      <c r="A233" s="7" t="s">
+      <c r="A233" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B233" s="7" t="s">
+      <c r="B233" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C233" s="8">
+      <c r="C233" s="9">
         <v>2.0</v>
       </c>
-      <c r="D233" s="8">
+      <c r="D233" s="9">
         <v>1.0</v>
       </c>
-      <c r="E233" s="7" t="s">
+      <c r="E233" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="F233" s="7" t="s">
+      <c r="F233" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="G233" s="9"/>
-      <c r="H233" s="8">
+      <c r="G233" s="10"/>
+      <c r="H233" s="9">
         <v>70.0</v>
       </c>
-      <c r="I233" s="8">
+      <c r="I233" s="9">
         <v>592.0</v>
       </c>
-      <c r="J233" s="8">
+      <c r="J233" s="9">
         <v>0.52</v>
       </c>
       <c r="K233" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Geochloa </v>
       </c>
-      <c r="L233" s="10"/>
-      <c r="M233" s="10"/>
-      <c r="N233" s="10"/>
-      <c r="O233" s="10"/>
-      <c r="P233" s="10"/>
-      <c r="Q233" s="10"/>
-      <c r="R233" s="10"/>
-      <c r="S233" s="10"/>
-      <c r="T233" s="10"/>
-      <c r="U233" s="10"/>
-      <c r="V233" s="10"/>
-      <c r="W233" s="10"/>
-      <c r="X233" s="10"/>
-      <c r="Y233" s="10"/>
-      <c r="Z233" s="10"/>
-      <c r="AA233" s="10"/>
+      <c r="L233" s="11"/>
+      <c r="M233" s="11"/>
+      <c r="N233" s="11"/>
+      <c r="O233" s="11"/>
+      <c r="P233" s="11"/>
+      <c r="Q233" s="11"/>
+      <c r="R233" s="11"/>
+      <c r="S233" s="11"/>
+      <c r="T233" s="11"/>
+      <c r="U233" s="11"/>
+      <c r="V233" s="11"/>
+      <c r="W233" s="11"/>
+      <c r="X233" s="11"/>
+      <c r="Y233" s="11"/>
+      <c r="Z233" s="11"/>
+      <c r="AA233" s="11"/>
     </row>
     <row r="234">
-      <c r="A234" s="7" t="s">
+      <c r="A234" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B234" s="7" t="s">
+      <c r="B234" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C234" s="8">
+      <c r="C234" s="9">
         <v>2.0</v>
       </c>
-      <c r="D234" s="8">
+      <c r="D234" s="9">
         <v>2.0</v>
       </c>
-      <c r="E234" s="7" t="s">
+      <c r="E234" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="F234" s="7" t="s">
+      <c r="F234" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="G234" s="9"/>
-      <c r="H234" s="8">
+      <c r="G234" s="10"/>
+      <c r="H234" s="9">
         <v>74.0</v>
       </c>
-      <c r="I234" s="8">
+      <c r="I234" s="9">
         <v>607.0</v>
       </c>
-      <c r="J234" s="8">
+      <c r="J234" s="9">
         <v>0.79</v>
       </c>
       <c r="K234" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Geochloa </v>
       </c>
-      <c r="L234" s="10"/>
-      <c r="M234" s="10"/>
-      <c r="N234" s="10"/>
-      <c r="O234" s="10"/>
-      <c r="P234" s="10"/>
-      <c r="Q234" s="10"/>
-      <c r="R234" s="10"/>
-      <c r="S234" s="10"/>
-      <c r="T234" s="10"/>
-      <c r="U234" s="10"/>
-      <c r="V234" s="10"/>
-      <c r="W234" s="10"/>
-      <c r="X234" s="10"/>
-      <c r="Y234" s="10"/>
-      <c r="Z234" s="10"/>
-      <c r="AA234" s="10"/>
+      <c r="L234" s="11"/>
+      <c r="M234" s="11"/>
+      <c r="N234" s="11"/>
+      <c r="O234" s="11"/>
+      <c r="P234" s="11"/>
+      <c r="Q234" s="11"/>
+      <c r="R234" s="11"/>
+      <c r="S234" s="11"/>
+      <c r="T234" s="11"/>
+      <c r="U234" s="11"/>
+      <c r="V234" s="11"/>
+      <c r="W234" s="11"/>
+      <c r="X234" s="11"/>
+      <c r="Y234" s="11"/>
+      <c r="Z234" s="11"/>
+      <c r="AA234" s="11"/>
     </row>
     <row r="235">
-      <c r="A235" s="7" t="s">
+      <c r="A235" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B235" s="7" t="s">
+      <c r="B235" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C235" s="8">
+      <c r="C235" s="9">
         <v>2.0</v>
       </c>
-      <c r="D235" s="8">
+      <c r="D235" s="9">
         <v>3.0</v>
       </c>
-      <c r="E235" s="7" t="s">
+      <c r="E235" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="F235" s="7" t="s">
+      <c r="F235" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="G235" s="9"/>
-      <c r="H235" s="8">
+      <c r="G235" s="10"/>
+      <c r="H235" s="9">
         <v>100.0</v>
       </c>
-      <c r="I235" s="8">
+      <c r="I235" s="9">
         <v>570.0</v>
       </c>
-      <c r="J235" s="8">
+      <c r="J235" s="9">
         <v>0.61</v>
       </c>
       <c r="K235" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Geochloa </v>
       </c>
-      <c r="L235" s="10"/>
-      <c r="M235" s="10"/>
-      <c r="N235" s="10"/>
-      <c r="O235" s="10"/>
-      <c r="P235" s="10"/>
-      <c r="Q235" s="10"/>
-      <c r="R235" s="10"/>
-      <c r="S235" s="10"/>
-      <c r="T235" s="10"/>
-      <c r="U235" s="10"/>
-      <c r="V235" s="10"/>
-      <c r="W235" s="10"/>
-      <c r="X235" s="10"/>
-      <c r="Y235" s="10"/>
-      <c r="Z235" s="10"/>
-      <c r="AA235" s="10"/>
+      <c r="L235" s="11"/>
+      <c r="M235" s="11"/>
+      <c r="N235" s="11"/>
+      <c r="O235" s="11"/>
+      <c r="P235" s="11"/>
+      <c r="Q235" s="11"/>
+      <c r="R235" s="11"/>
+      <c r="S235" s="11"/>
+      <c r="T235" s="11"/>
+      <c r="U235" s="11"/>
+      <c r="V235" s="11"/>
+      <c r="W235" s="11"/>
+      <c r="X235" s="11"/>
+      <c r="Y235" s="11"/>
+      <c r="Z235" s="11"/>
+      <c r="AA235" s="11"/>
     </row>
     <row r="236">
       <c r="A236" s="2" t="s">
@@ -27713,7 +27769,7 @@
       <c r="F245" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G245" s="4"/>
+      <c r="G245" s="7"/>
       <c r="H245" s="3">
         <v>53.0</v>
       </c>
@@ -27747,7 +27803,7 @@
       <c r="F246" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G246" s="4"/>
+      <c r="G246" s="7"/>
       <c r="H246" s="3">
         <v>57.0</v>
       </c>
@@ -27781,7 +27837,7 @@
       <c r="F247" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G247" s="4"/>
+      <c r="G247" s="7"/>
       <c r="H247" s="3">
         <v>44.0</v>
       </c>
@@ -27797,310 +27853,310 @@
       </c>
     </row>
     <row r="248">
-      <c r="A248" s="7" t="s">
+      <c r="A248" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B248" s="7" t="s">
+      <c r="B248" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C248" s="8">
+      <c r="C248" s="9">
         <v>4.0</v>
       </c>
-      <c r="D248" s="8">
+      <c r="D248" s="9">
         <v>1.0</v>
       </c>
-      <c r="E248" s="7" t="s">
+      <c r="E248" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="F248" s="11" t="s">
+      <c r="F248" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="G248" s="11" t="s">
+      <c r="G248" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="H248" s="8">
+      <c r="H248" s="9">
         <v>15.0</v>
       </c>
-      <c r="I248" s="8">
+      <c r="I248" s="9">
         <v>10.32</v>
       </c>
-      <c r="J248" s="8">
+      <c r="J248" s="9">
         <v>1.5</v>
       </c>
       <c r="K248" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Trifolium angustifolium</v>
       </c>
-      <c r="L248" s="10"/>
-      <c r="M248" s="10"/>
-      <c r="N248" s="10"/>
-      <c r="O248" s="10"/>
-      <c r="P248" s="10"/>
-      <c r="Q248" s="10"/>
-      <c r="R248" s="10"/>
-      <c r="S248" s="10"/>
-      <c r="T248" s="10"/>
-      <c r="U248" s="10"/>
-      <c r="V248" s="10"/>
-      <c r="W248" s="10"/>
-      <c r="X248" s="10"/>
-      <c r="Y248" s="10"/>
-      <c r="Z248" s="10"/>
-      <c r="AA248" s="10"/>
+      <c r="L248" s="11"/>
+      <c r="M248" s="11"/>
+      <c r="N248" s="11"/>
+      <c r="O248" s="11"/>
+      <c r="P248" s="11"/>
+      <c r="Q248" s="11"/>
+      <c r="R248" s="11"/>
+      <c r="S248" s="11"/>
+      <c r="T248" s="11"/>
+      <c r="U248" s="11"/>
+      <c r="V248" s="11"/>
+      <c r="W248" s="11"/>
+      <c r="X248" s="11"/>
+      <c r="Y248" s="11"/>
+      <c r="Z248" s="11"/>
+      <c r="AA248" s="11"/>
     </row>
     <row r="249">
-      <c r="A249" s="7" t="s">
+      <c r="A249" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B249" s="7" t="s">
+      <c r="B249" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C249" s="8">
+      <c r="C249" s="9">
         <v>4.0</v>
       </c>
-      <c r="D249" s="8">
+      <c r="D249" s="9">
         <v>2.0</v>
       </c>
-      <c r="E249" s="7" t="s">
+      <c r="E249" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="F249" s="11" t="s">
+      <c r="F249" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="G249" s="11" t="s">
+      <c r="G249" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="H249" s="8">
+      <c r="H249" s="9">
         <v>17.0</v>
       </c>
-      <c r="I249" s="8">
+      <c r="I249" s="9">
         <v>10.25</v>
       </c>
-      <c r="J249" s="8">
+      <c r="J249" s="9">
         <v>1.29</v>
       </c>
       <c r="K249" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Trifolium angustifolium</v>
       </c>
-      <c r="L249" s="10"/>
-      <c r="M249" s="10"/>
-      <c r="N249" s="10"/>
-      <c r="O249" s="10"/>
-      <c r="P249" s="10"/>
-      <c r="Q249" s="10"/>
-      <c r="R249" s="10"/>
-      <c r="S249" s="10"/>
-      <c r="T249" s="10"/>
-      <c r="U249" s="10"/>
-      <c r="V249" s="10"/>
-      <c r="W249" s="10"/>
-      <c r="X249" s="10"/>
-      <c r="Y249" s="10"/>
-      <c r="Z249" s="10"/>
-      <c r="AA249" s="10"/>
+      <c r="L249" s="11"/>
+      <c r="M249" s="11"/>
+      <c r="N249" s="11"/>
+      <c r="O249" s="11"/>
+      <c r="P249" s="11"/>
+      <c r="Q249" s="11"/>
+      <c r="R249" s="11"/>
+      <c r="S249" s="11"/>
+      <c r="T249" s="11"/>
+      <c r="U249" s="11"/>
+      <c r="V249" s="11"/>
+      <c r="W249" s="11"/>
+      <c r="X249" s="11"/>
+      <c r="Y249" s="11"/>
+      <c r="Z249" s="11"/>
+      <c r="AA249" s="11"/>
     </row>
     <row r="250">
-      <c r="A250" s="7" t="s">
+      <c r="A250" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B250" s="7" t="s">
+      <c r="B250" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C250" s="8">
+      <c r="C250" s="9">
         <v>4.0</v>
       </c>
-      <c r="D250" s="8">
+      <c r="D250" s="9">
         <v>3.0</v>
       </c>
-      <c r="E250" s="7" t="s">
+      <c r="E250" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="F250" s="11" t="s">
+      <c r="F250" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="G250" s="11" t="s">
+      <c r="G250" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="H250" s="8">
+      <c r="H250" s="9">
         <v>25.0</v>
       </c>
-      <c r="I250" s="8">
+      <c r="I250" s="9">
         <v>8.41</v>
       </c>
-      <c r="J250" s="8">
+      <c r="J250" s="9">
         <v>2.12</v>
       </c>
       <c r="K250" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Trifolium angustifolium</v>
       </c>
-      <c r="L250" s="10"/>
-      <c r="M250" s="10"/>
-      <c r="N250" s="10"/>
-      <c r="O250" s="10"/>
-      <c r="P250" s="10"/>
-      <c r="Q250" s="10"/>
-      <c r="R250" s="10"/>
-      <c r="S250" s="10"/>
-      <c r="T250" s="10"/>
-      <c r="U250" s="10"/>
-      <c r="V250" s="10"/>
-      <c r="W250" s="10"/>
-      <c r="X250" s="10"/>
-      <c r="Y250" s="10"/>
-      <c r="Z250" s="10"/>
-      <c r="AA250" s="10"/>
+      <c r="L250" s="11"/>
+      <c r="M250" s="11"/>
+      <c r="N250" s="11"/>
+      <c r="O250" s="11"/>
+      <c r="P250" s="11"/>
+      <c r="Q250" s="11"/>
+      <c r="R250" s="11"/>
+      <c r="S250" s="11"/>
+      <c r="T250" s="11"/>
+      <c r="U250" s="11"/>
+      <c r="V250" s="11"/>
+      <c r="W250" s="11"/>
+      <c r="X250" s="11"/>
+      <c r="Y250" s="11"/>
+      <c r="Z250" s="11"/>
+      <c r="AA250" s="11"/>
     </row>
     <row r="251">
-      <c r="A251" s="7" t="s">
+      <c r="A251" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B251" s="7" t="s">
+      <c r="B251" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C251" s="8">
+      <c r="C251" s="9">
         <v>5.0</v>
       </c>
-      <c r="D251" s="8">
+      <c r="D251" s="9">
         <v>1.0</v>
       </c>
-      <c r="E251" s="7" t="s">
+      <c r="E251" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="F251" s="7" t="s">
+      <c r="F251" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="G251" s="9"/>
-      <c r="H251" s="8">
+      <c r="G251" s="10"/>
+      <c r="H251" s="9">
         <v>46.0</v>
       </c>
-      <c r="I251" s="8">
+      <c r="I251" s="9">
         <v>8.26</v>
       </c>
-      <c r="J251" s="8">
+      <c r="J251" s="9">
         <v>1.51</v>
       </c>
       <c r="K251" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Tricusperdatum </v>
       </c>
-      <c r="L251" s="10"/>
-      <c r="M251" s="10"/>
-      <c r="N251" s="10"/>
-      <c r="O251" s="10"/>
-      <c r="P251" s="10"/>
-      <c r="Q251" s="10"/>
-      <c r="R251" s="10"/>
-      <c r="S251" s="10"/>
-      <c r="T251" s="10"/>
-      <c r="U251" s="10"/>
-      <c r="V251" s="10"/>
-      <c r="W251" s="10"/>
-      <c r="X251" s="10"/>
-      <c r="Y251" s="10"/>
-      <c r="Z251" s="10"/>
-      <c r="AA251" s="10"/>
+      <c r="L251" s="11"/>
+      <c r="M251" s="11"/>
+      <c r="N251" s="11"/>
+      <c r="O251" s="11"/>
+      <c r="P251" s="11"/>
+      <c r="Q251" s="11"/>
+      <c r="R251" s="11"/>
+      <c r="S251" s="11"/>
+      <c r="T251" s="11"/>
+      <c r="U251" s="11"/>
+      <c r="V251" s="11"/>
+      <c r="W251" s="11"/>
+      <c r="X251" s="11"/>
+      <c r="Y251" s="11"/>
+      <c r="Z251" s="11"/>
+      <c r="AA251" s="11"/>
     </row>
     <row r="252">
-      <c r="A252" s="7" t="s">
+      <c r="A252" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B252" s="7" t="s">
+      <c r="B252" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C252" s="8">
+      <c r="C252" s="9">
         <v>5.0</v>
       </c>
-      <c r="D252" s="8">
+      <c r="D252" s="9">
         <v>2.0</v>
       </c>
-      <c r="E252" s="7" t="s">
+      <c r="E252" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="F252" s="7" t="s">
+      <c r="F252" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="G252" s="9"/>
-      <c r="H252" s="8">
+      <c r="G252" s="10"/>
+      <c r="H252" s="9">
         <v>46.0</v>
       </c>
-      <c r="I252" s="8">
+      <c r="I252" s="9">
         <v>9.05</v>
       </c>
-      <c r="J252" s="8">
+      <c r="J252" s="9">
         <v>1.34</v>
       </c>
       <c r="K252" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Tricusperdatum </v>
       </c>
-      <c r="L252" s="10"/>
-      <c r="M252" s="10"/>
-      <c r="N252" s="10"/>
-      <c r="O252" s="10"/>
-      <c r="P252" s="10"/>
-      <c r="Q252" s="10"/>
-      <c r="R252" s="10"/>
-      <c r="S252" s="10"/>
-      <c r="T252" s="10"/>
-      <c r="U252" s="10"/>
-      <c r="V252" s="10"/>
-      <c r="W252" s="10"/>
-      <c r="X252" s="10"/>
-      <c r="Y252" s="10"/>
-      <c r="Z252" s="10"/>
-      <c r="AA252" s="10"/>
+      <c r="L252" s="11"/>
+      <c r="M252" s="11"/>
+      <c r="N252" s="11"/>
+      <c r="O252" s="11"/>
+      <c r="P252" s="11"/>
+      <c r="Q252" s="11"/>
+      <c r="R252" s="11"/>
+      <c r="S252" s="11"/>
+      <c r="T252" s="11"/>
+      <c r="U252" s="11"/>
+      <c r="V252" s="11"/>
+      <c r="W252" s="11"/>
+      <c r="X252" s="11"/>
+      <c r="Y252" s="11"/>
+      <c r="Z252" s="11"/>
+      <c r="AA252" s="11"/>
     </row>
     <row r="253">
-      <c r="A253" s="7" t="s">
+      <c r="A253" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B253" s="7" t="s">
+      <c r="B253" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C253" s="8">
+      <c r="C253" s="9">
         <v>5.0</v>
       </c>
-      <c r="D253" s="8">
+      <c r="D253" s="9">
         <v>3.0</v>
       </c>
-      <c r="E253" s="7" t="s">
+      <c r="E253" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="F253" s="7" t="s">
+      <c r="F253" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="G253" s="9"/>
-      <c r="H253" s="8">
+      <c r="G253" s="10"/>
+      <c r="H253" s="9">
         <v>31.0</v>
       </c>
-      <c r="I253" s="8">
+      <c r="I253" s="9">
         <v>7.5</v>
       </c>
-      <c r="J253" s="8">
+      <c r="J253" s="9">
         <v>1.6</v>
       </c>
       <c r="K253" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Tricusperdatum </v>
       </c>
-      <c r="L253" s="10"/>
-      <c r="M253" s="10"/>
-      <c r="N253" s="10"/>
-      <c r="O253" s="10"/>
-      <c r="P253" s="10"/>
-      <c r="Q253" s="10"/>
-      <c r="R253" s="10"/>
-      <c r="S253" s="10"/>
-      <c r="T253" s="10"/>
-      <c r="U253" s="10"/>
-      <c r="V253" s="10"/>
-      <c r="W253" s="10"/>
-      <c r="X253" s="10"/>
-      <c r="Y253" s="10"/>
-      <c r="Z253" s="10"/>
-      <c r="AA253" s="10"/>
+      <c r="L253" s="11"/>
+      <c r="M253" s="11"/>
+      <c r="N253" s="11"/>
+      <c r="O253" s="11"/>
+      <c r="P253" s="11"/>
+      <c r="Q253" s="11"/>
+      <c r="R253" s="11"/>
+      <c r="S253" s="11"/>
+      <c r="T253" s="11"/>
+      <c r="U253" s="11"/>
+      <c r="V253" s="11"/>
+      <c r="W253" s="11"/>
+      <c r="X253" s="11"/>
+      <c r="Y253" s="11"/>
+      <c r="Z253" s="11"/>
+      <c r="AA253" s="11"/>
     </row>
     <row r="254">
       <c r="A254" s="2" t="s">
@@ -28877,7 +28933,7 @@
       <c r="F275" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="G275" s="4"/>
+      <c r="G275" s="7"/>
       <c r="H275" s="3">
         <v>132.0</v>
       </c>
@@ -28911,7 +28967,7 @@
       <c r="F276" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="G276" s="4"/>
+      <c r="G276" s="7"/>
       <c r="H276" s="3">
         <v>91.0</v>
       </c>
@@ -28945,7 +29001,7 @@
       <c r="F277" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="G277" s="4"/>
+      <c r="G277" s="7"/>
       <c r="H277" s="3">
         <v>130.0</v>
       </c>
@@ -29297,7 +29353,7 @@
       <c r="F287" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G287" s="4"/>
+      <c r="G287" s="7"/>
       <c r="H287" s="3">
         <v>113.0</v>
       </c>
@@ -29331,7 +29387,7 @@
       <c r="F288" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G288" s="4"/>
+      <c r="G288" s="7"/>
       <c r="H288" s="3">
         <v>102.0</v>
       </c>
@@ -29365,7 +29421,7 @@
       <c r="F289" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G289" s="4"/>
+      <c r="G289" s="7"/>
       <c r="H289" s="3">
         <v>96.0</v>
       </c>
@@ -29507,7 +29563,7 @@
       <c r="F293" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G293" s="4"/>
+      <c r="G293" s="7"/>
       <c r="H293" s="3">
         <v>55.0</v>
       </c>
@@ -29541,7 +29597,7 @@
       <c r="F294" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G294" s="4"/>
+      <c r="G294" s="7"/>
       <c r="H294" s="3">
         <v>65.0</v>
       </c>
@@ -29575,7 +29631,7 @@
       <c r="F295" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G295" s="4"/>
+      <c r="G295" s="7"/>
       <c r="H295" s="3">
         <v>74.0</v>
       </c>
@@ -31373,10 +31429,10 @@
       <c r="D71" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E71" s="13" t="s">
+      <c r="E71" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="F71" s="13" t="s">
+      <c r="F71" s="14" t="s">
         <v>161</v>
       </c>
       <c r="H71" s="6" t="str">
@@ -32472,10 +32528,10 @@
       <c r="D115" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E115" s="13" t="s">
+      <c r="E115" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F115" s="13" t="s">
+      <c r="F115" s="14" t="s">
         <v>53</v>
       </c>
       <c r="H115" s="6" t="str">

</xml_diff>